<commit_message>
Modificando por un archivo en Excel ESPANHOL
Los separadores de funciones son ";" y no ","
</commit_message>
<xml_diff>
--- a/public/Uploads/Recursos/temp-administra-docentes.xlsx
+++ b/public/Uploads/Recursos/temp-administra-docentes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eramirez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="docentes" sheetId="1" r:id="rId1"/>
     <sheet name="info" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="catalogos" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -331,6 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -408,22 +409,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="cargos" displayName="cargos" ref="A1:B10" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="cargos" displayName="cargos" ref="A1:B10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:B10"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CARGO"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID"/>
+    <tableColumn id="1" name="CARGO"/>
+    <tableColumn id="2" name="ID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="jornadas" displayName="jornadas" ref="D1:E4" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="D1:E4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="jornadas" displayName="jornadas" ref="D1:E4" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D1:E4"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="JORNADA"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID"/>
+    <tableColumn id="1" name="JORNADA"/>
+    <tableColumn id="2" name="ID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -691,22 +692,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="7" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.5546875" style="7" customWidth="1"/>
-    <col min="7" max="8" width="39.88671875" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" style="7"/>
+    <col min="2" max="2" width="22.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.5703125" style="7" customWidth="1"/>
+    <col min="7" max="8" width="39.85546875" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -720,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -728,318 +731,324 @@
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="9"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="caPMEPiV/oAyqIDjYQ8kFjxZWA0yWyTnPqB7LQxZQw2kqSvUbcQqeZFGasIylNBtyfwF/SzSl+41wkNoRpb0bw==" saltValue="LjKei7+fhMGAnhKSmfeAGA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="IhXttetCbpJniOtW4p5ZlmrVmiOXxN5RASuwLzdAhsX62h7Ck4SpdQAGmvxKeb+Gby5im1NovbUjdA6Utz5mTg==" saltValue="Mrh5D5g/Zy1hXtjHmCqTmA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="6">
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G7:H7"/>
@@ -1049,27 +1058,26 @@
     <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Jornada" prompt="Seleccione un tipo de jornada para el docente. Este campo es obligatorio." xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Jornada" prompt="Seleccione un tipo de jornada para el docente. Este campo es obligatorio.">
           <x14:formula1>
             <xm:f>catalogos!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B49</xm:sqref>
+          <xm:sqref>B2:B51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Cargo Secundario" prompt="Seleccione un cargo secundario para el docente. Este campo es opcional." xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Cargo Secundario" prompt="Seleccione un cargo secundario para el docente. Este campo es opcional.">
           <x14:formula1>
             <xm:f>catalogos!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D49</xm:sqref>
+          <xm:sqref>D2:D51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Cargo Principal" prompt="Seleccione un cargo principal para el docente. Este campo es obligatorio." xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Cargo Principal" prompt="Seleccione un cargo principal para el docente. Este campo es obligatorio.">
           <x14:formula1>
             <xm:f>catalogos!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C49</xm:sqref>
+          <xm:sqref>C2:C51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1078,16 +1086,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1101,14 +1109,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(docentes!A2="","",docentes!A2)</f>
         <v>user1</v>
       </c>
       <c r="B2" s="2">
         <f>IFERROR(VLOOKUP(docentes!C2,cargos[],2,FALSE),"")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <f>IFERROR(VLOOKUP(docentes!D2,cargos[],2,FALSE),"")</f>
@@ -1119,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>IF(docentes!A3="","",docentes!A3)</f>
         <v/>
@@ -1137,7 +1145,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>IF(docentes!A4="","",docentes!A4)</f>
         <v/>
@@ -1155,7 +1163,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>IF(docentes!A5="","",docentes!A5)</f>
         <v/>
@@ -1173,7 +1181,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>IF(docentes!A6="","",docentes!A6)</f>
         <v/>
@@ -1191,7 +1199,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>IF(docentes!A7="","",docentes!A7)</f>
         <v/>
@@ -1209,7 +1217,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>IF(docentes!A8="","",docentes!A8)</f>
         <v/>
@@ -1227,7 +1235,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f>IF(docentes!A9="","",docentes!A9)</f>
         <v/>
@@ -1245,7 +1253,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
         <f>IF(docentes!A10="","",docentes!A10)</f>
         <v/>
@@ -1263,7 +1271,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f>IF(docentes!A11="","",docentes!A11)</f>
         <v/>
@@ -1281,7 +1289,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f>IF(docentes!A12="","",docentes!A12)</f>
         <v/>
@@ -1299,7 +1307,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
         <f>IF(docentes!A13="","",docentes!A13)</f>
         <v/>
@@ -1317,7 +1325,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>IF(docentes!A14="","",docentes!A14)</f>
         <v/>
@@ -1335,7 +1343,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>IF(docentes!A15="","",docentes!A15)</f>
         <v/>
@@ -1353,7 +1361,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>IF(docentes!A16="","",docentes!A16)</f>
         <v/>
@@ -1371,7 +1379,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f>IF(docentes!A17="","",docentes!A17)</f>
         <v/>
@@ -1389,7 +1397,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>IF(docentes!A18="","",docentes!A18)</f>
         <v/>
@@ -1407,7 +1415,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f>IF(docentes!A19="","",docentes!A19)</f>
         <v/>
@@ -1425,7 +1433,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f>IF(docentes!A20="","",docentes!A20)</f>
         <v/>
@@ -1443,7 +1451,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f>IF(docentes!A21="","",docentes!A21)</f>
         <v/>
@@ -1461,7 +1469,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f>IF(docentes!A22="","",docentes!A22)</f>
         <v/>
@@ -1479,7 +1487,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f>IF(docentes!A23="","",docentes!A23)</f>
         <v/>
@@ -1497,7 +1505,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f>IF(docentes!A24="","",docentes!A24)</f>
         <v/>
@@ -1515,7 +1523,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f>IF(docentes!A25="","",docentes!A25)</f>
         <v/>
@@ -1533,7 +1541,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f>IF(docentes!A26="","",docentes!A26)</f>
         <v/>
@@ -1551,7 +1559,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f>IF(docentes!A27="","",docentes!A27)</f>
         <v/>
@@ -1569,7 +1577,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="str">
         <f>IF(docentes!A28="","",docentes!A28)</f>
         <v/>
@@ -1587,7 +1595,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="str">
         <f>IF(docentes!A29="","",docentes!A29)</f>
         <v/>
@@ -1605,7 +1613,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="str">
         <f>IF(docentes!A30="","",docentes!A30)</f>
         <v/>
@@ -1623,7 +1631,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="str">
         <f>IF(docentes!A31="","",docentes!A31)</f>
         <v/>
@@ -1641,7 +1649,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="str">
         <f>IF(docentes!A32="","",docentes!A32)</f>
         <v/>
@@ -1659,7 +1667,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="str">
         <f>IF(docentes!A33="","",docentes!A33)</f>
         <v/>
@@ -1677,7 +1685,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="str">
         <f>IF(docentes!A34="","",docentes!A34)</f>
         <v/>
@@ -1695,7 +1703,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="str">
         <f>IF(docentes!A35="","",docentes!A35)</f>
         <v/>
@@ -1713,7 +1721,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="str">
         <f>IF(docentes!A36="","",docentes!A36)</f>
         <v/>
@@ -1731,7 +1739,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="str">
         <f>IF(docentes!A37="","",docentes!A37)</f>
         <v/>
@@ -1749,7 +1757,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="str">
         <f>IF(docentes!A38="","",docentes!A38)</f>
         <v/>
@@ -1767,7 +1775,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="str">
         <f>IF(docentes!A39="","",docentes!A39)</f>
         <v/>
@@ -1785,7 +1793,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="str">
         <f>IF(docentes!A40="","",docentes!A40)</f>
         <v/>
@@ -1803,7 +1811,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="str">
         <f>IF(docentes!A41="","",docentes!A41)</f>
         <v/>
@@ -1821,7 +1829,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="str">
         <f>IF(docentes!A42="","",docentes!A42)</f>
         <v/>
@@ -1839,7 +1847,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="str">
         <f>IF(docentes!A43="","",docentes!A43)</f>
         <v/>
@@ -1857,7 +1865,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="str">
         <f>IF(docentes!A44="","",docentes!A44)</f>
         <v/>
@@ -1875,7 +1883,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="str">
         <f>IF(docentes!A45="","",docentes!A45)</f>
         <v/>
@@ -1893,7 +1901,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="str">
         <f>IF(docentes!A46="","",docentes!A46)</f>
         <v/>
@@ -1911,7 +1919,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="str">
         <f>IF(docentes!A47="","",docentes!A47)</f>
         <v/>
@@ -1929,7 +1937,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="str">
         <f>IF(docentes!A48="","",docentes!A48)</f>
         <v/>
@@ -1947,7 +1955,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="str">
         <f>IF(docentes!A49="","",docentes!A49)</f>
         <v/>
@@ -1965,21 +1973,21 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="e">
-        <f>IF(docentes!#REF!="","",docentes!#REF!)</f>
-        <v>#REF!</v>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="str">
+        <f>IF(docentes!A50="","",docentes!A50)</f>
+        <v/>
       </c>
       <c r="B50" s="2" t="str">
-        <f>IFERROR(VLOOKUP(docentes!#REF!,cargos[],2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(docentes!C50,cargos[],2,FALSE),"")</f>
         <v/>
       </c>
       <c r="C50" s="2" t="str">
-        <f>IFERROR(VLOOKUP(docentes!#REF!,cargos[],2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(docentes!D50,cargos[],2,FALSE),"")</f>
         <v/>
       </c>
       <c r="D50" s="2" t="str">
-        <f>IFERROR(VLOOKUP(docentes!#REF!,jornadas[],2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(docentes!B50,jornadas[],2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -1991,20 +1999,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -2018,7 +2026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2032,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2046,7 +2054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2060,7 +2068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2068,7 +2076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2076,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2084,7 +2092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2092,7 +2100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2100,7 +2108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>

</xml_diff>